<commit_message>
update website with all sta
</commit_message>
<xml_diff>
--- a/data/gpr_settings.xlsx
+++ b/data/gpr_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael/Library/CloudStorage/Box-Box/Val-Piora-Wheatear/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBF8C9B-A96F-6041-AB98-F1045239812D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD6C653-9904-C24D-B34F-95E555B6F248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="500" windowWidth="27660" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="500" yWindow="500" windowWidth="27660" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tracks" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="63">
   <si>
     <t>Color</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>kernel_adjust</t>
+  </si>
+  <si>
+    <t>keep</t>
   </si>
 </sst>
 </file>
@@ -863,13 +866,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}" name="Table1" displayName="Table1" ref="A1:AG15" totalsRowShown="0">
-  <autoFilter ref="A1:AG15" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AG15">
-    <sortCondition ref="U1:U15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}" name="Table1" displayName="Table1" ref="A1:AH15" totalsRowShown="0">
+  <autoFilter ref="A1:AH15" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AH15">
+    <sortCondition ref="V1:V15"/>
   </sortState>
-  <tableColumns count="33">
+  <tableColumns count="34">
     <tableColumn id="3" xr3:uid="{0E08F938-60A9-C640-A060-C64653A1D0F0}" name="gdl_id" dataDxfId="14" dataCellStyle="Normal_Feuil1"/>
+    <tableColumn id="12" xr3:uid="{A35DC4F6-C589-EF4B-8615-0E1885154BE5}" name="keep"/>
     <tableColumn id="38" xr3:uid="{5F80A124-B607-6D47-A8B2-B6EBC16D0EC2}" name="crop_start" dataDxfId="13"/>
     <tableColumn id="39" xr3:uid="{C4B8ED7B-88BE-D143-A9A5-6213689753CA}" name="crop_end" dataDxfId="12"/>
     <tableColumn id="6" xr3:uid="{22680B6F-F907-FD43-BF6C-2E3789C9C356}" name="thr_dur" dataDxfId="11"/>
@@ -1204,1298 +1208,1343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG15"/>
+  <dimension ref="A1:AH15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A15"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="12" max="12" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" customWidth="1"/>
-    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="15.1640625" customWidth="1"/>
-    <col min="18" max="18" width="18.83203125" customWidth="1"/>
-    <col min="19" max="19" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.1640625" customWidth="1"/>
-    <col min="22" max="22" width="14.1640625" customWidth="1"/>
-    <col min="23" max="27" width="17.33203125" customWidth="1"/>
-    <col min="29" max="29" width="17.33203125" customWidth="1"/>
-    <col min="30" max="30" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.5" customWidth="1"/>
-    <col min="37" max="37" width="16.33203125" customWidth="1"/>
-    <col min="43" max="45" width="15.1640625" customWidth="1"/>
-    <col min="46" max="46" width="14.5" customWidth="1"/>
-    <col min="47" max="47" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="18" customWidth="1"/>
+    <col min="18" max="18" width="15.1640625" customWidth="1"/>
+    <col min="19" max="19" width="18.83203125" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.1640625" customWidth="1"/>
+    <col min="23" max="23" width="14.1640625" customWidth="1"/>
+    <col min="24" max="28" width="17.33203125" customWidth="1"/>
+    <col min="30" max="30" width="17.33203125" customWidth="1"/>
+    <col min="31" max="31" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5" customWidth="1"/>
+    <col min="38" max="38" width="16.33203125" customWidth="1"/>
+    <col min="44" max="46" width="15.1640625" customWidth="1"/>
+    <col min="47" max="47" width="14.5" customWidth="1"/>
+    <col min="48" max="48" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>22</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>60</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>26</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>61</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>8</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>9</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>13</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>14</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>15</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>16</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>27</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>29</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>30</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>2</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>5</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>1</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>6</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1">
         <v>44026</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>44344</v>
       </c>
-      <c r="D2" s="3">
-        <v>24</v>
-      </c>
-      <c r="E2">
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>51</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>-18</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>4</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>16</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>5</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>300</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>30</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>1</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>2</v>
       </c>
-      <c r="N2">
-        <v>0.9</v>
-      </c>
       <c r="O2">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
         <v>1.4</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>8.7055030000000002</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>46.550758000000002</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="1">
         <v>44026</v>
       </c>
-      <c r="T2" s="1">
+      <c r="U2" s="1">
         <v>44091</v>
       </c>
-      <c r="U2" s="1">
+      <c r="V2" s="1">
         <v>44319</v>
       </c>
-      <c r="V2" s="1">
+      <c r="W2" s="1">
         <v>44344</v>
       </c>
-      <c r="W2" s="1"/>
       <c r="X2" s="1"/>
-      <c r="Y2" s="3">
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="3">
         <v>0.1</v>
       </c>
-      <c r="Z2" s="3">
-        <v>0.9</v>
-      </c>
       <c r="AA2" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AB2" s="3">
         <v>120</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>54</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>58</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
         <v>44026</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>44377</v>
       </c>
-      <c r="D3" s="3">
-        <v>24</v>
-      </c>
-      <c r="E3">
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>51</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>-18</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>4</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>16</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>5</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>300</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>30</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>1</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>2</v>
       </c>
-      <c r="N3">
-        <v>0.9</v>
-      </c>
       <c r="O3">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
         <v>1.4</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>8.7060300000000002</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>46.549204000000003</v>
       </c>
-      <c r="S3" s="1">
+      <c r="T3" s="1">
         <v>44026</v>
       </c>
-      <c r="T3" s="1">
+      <c r="U3" s="1">
         <v>44085</v>
       </c>
-      <c r="U3" s="1">
+      <c r="V3" s="1">
         <v>44324</v>
       </c>
-      <c r="V3" s="1">
+      <c r="W3" s="1">
         <v>44377</v>
       </c>
-      <c r="W3" s="1"/>
       <c r="X3" s="1"/>
-      <c r="Y3" s="3">
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="3">
         <v>0.1</v>
       </c>
-      <c r="Z3" s="3">
-        <v>0.9</v>
-      </c>
       <c r="AA3" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AB3" s="3">
         <v>120</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>52</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>58</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1">
         <v>44019</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>44370</v>
       </c>
-      <c r="D4" s="3">
-        <v>24</v>
-      </c>
-      <c r="E4">
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>51</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>-18</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>4</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>16</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>5</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>300</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>30</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>1</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>2</v>
       </c>
-      <c r="N4">
-        <v>0.9</v>
-      </c>
       <c r="O4">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
         <v>1.4</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>8.7117020000000007</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>46.553612999999999</v>
       </c>
-      <c r="S4" s="1">
+      <c r="T4" s="1">
         <v>44019</v>
       </c>
-      <c r="T4" s="1">
+      <c r="U4" s="1">
         <v>44091</v>
       </c>
-      <c r="U4" s="1">
+      <c r="V4" s="1">
         <v>44329</v>
       </c>
-      <c r="V4" s="1">
+      <c r="W4" s="1">
         <v>44370</v>
       </c>
-      <c r="W4" s="1"/>
       <c r="X4" s="1"/>
-      <c r="Y4" s="3">
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="3">
         <v>0.1</v>
       </c>
-      <c r="Z4" s="3">
-        <v>0.9</v>
-      </c>
       <c r="AA4" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AB4" s="3">
         <v>120</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>56</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>58</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1">
         <v>43666</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>43769.239583333336</v>
       </c>
-      <c r="D5" s="3">
-        <v>24</v>
-      </c>
-      <c r="E5">
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>51</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>-18</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>4</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>16</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>5</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>300</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>30</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>1</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>2</v>
       </c>
-      <c r="N5">
-        <v>0.9</v>
-      </c>
       <c r="O5">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
         <v>1.4</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>6.96333</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>44.951770000000003</v>
       </c>
-      <c r="S5" s="1">
+      <c r="T5" s="1">
         <v>43666</v>
       </c>
-      <c r="T5" s="1">
+      <c r="U5" s="1">
         <v>43724</v>
       </c>
-      <c r="W5" s="1"/>
       <c r="X5" s="1"/>
-      <c r="Y5" s="3">
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="3">
         <v>0.1</v>
       </c>
-      <c r="Z5" s="3">
-        <v>0.9</v>
-      </c>
       <c r="AA5" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AB5" s="3">
         <v>120</v>
       </c>
-      <c r="AB5" s="4" t="s">
+      <c r="AC5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>58</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>59</v>
       </c>
-      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
         <v>43666</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>43750.222222222219</v>
       </c>
-      <c r="D6" s="3">
-        <v>24</v>
-      </c>
-      <c r="E6">
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>51</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>-18</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>4</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>16</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>5</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>300</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>30</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>1</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>2</v>
       </c>
-      <c r="N6">
-        <v>0.9</v>
-      </c>
       <c r="O6">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
         <v>1.4</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>6.96333</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>44.951770000000003</v>
       </c>
-      <c r="S6" s="1">
+      <c r="T6" s="1">
         <v>43666</v>
       </c>
-      <c r="T6" s="1">
+      <c r="U6" s="1">
         <v>43720</v>
       </c>
-      <c r="W6" s="1"/>
       <c r="X6" s="1"/>
-      <c r="Y6" s="3">
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="3">
         <v>0.1</v>
       </c>
-      <c r="Z6" s="3">
-        <v>0.9</v>
-      </c>
       <c r="AA6" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AB6" s="3">
         <v>120</v>
       </c>
-      <c r="AB6" s="4" t="s">
+      <c r="AC6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>58</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
         <v>43666</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>43725.743055555555</v>
       </c>
-      <c r="D7" s="3">
-        <v>24</v>
-      </c>
-      <c r="E7">
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>51</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>-18</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>4</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>16</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>5</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>300</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>30</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>1</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>2</v>
       </c>
-      <c r="N7">
-        <v>0.9</v>
-      </c>
       <c r="O7">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
         <v>1.4</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>6.9699499999999999</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>44.953440000000001</v>
       </c>
-      <c r="S7" s="1">
+      <c r="T7" s="1">
         <v>43666</v>
       </c>
-      <c r="T7" s="1">
+      <c r="U7" s="1">
         <v>43714</v>
       </c>
-      <c r="W7" s="1"/>
       <c r="X7" s="1"/>
-      <c r="Y7" s="3">
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="3">
         <v>0.1</v>
       </c>
-      <c r="Z7" s="3">
-        <v>0.9</v>
-      </c>
       <c r="AA7" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AB7" s="3">
         <v>120</v>
       </c>
-      <c r="AB7" s="4" t="s">
+      <c r="AC7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>58</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1">
         <v>44043</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>44352</v>
       </c>
-      <c r="D8" s="3">
-        <v>24</v>
-      </c>
-      <c r="E8">
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>51</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>-18</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>4</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>16</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>5</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>300</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>30</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>1</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>2</v>
       </c>
-      <c r="N8">
-        <v>0.9</v>
-      </c>
       <c r="O8">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
         <v>1.4</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>6.9569460000000003</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>44.974710999999999</v>
       </c>
-      <c r="S8" s="1">
+      <c r="T8" s="1">
         <v>44043</v>
       </c>
-      <c r="T8" s="1">
+      <c r="U8" s="1">
         <v>44087</v>
       </c>
-      <c r="W8" s="1"/>
       <c r="X8" s="1"/>
-      <c r="Y8" s="3">
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="3">
         <v>0.1</v>
       </c>
-      <c r="Z8" s="3">
-        <v>0.9</v>
-      </c>
       <c r="AA8" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AB8" s="3">
         <v>120</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>58</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
         <v>42552</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>42763.756944444445</v>
       </c>
-      <c r="D9" s="3">
-        <v>24</v>
-      </c>
-      <c r="E9">
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>51</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>-18</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>4</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>16</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>5</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>300</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>30</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>1</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>2</v>
       </c>
-      <c r="N9">
-        <v>0.9</v>
-      </c>
       <c r="O9">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
         <v>1.4</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>8.6836400000000005</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>46.542700000000004</v>
       </c>
-      <c r="S9" s="1">
+      <c r="T9" s="1">
         <v>42552</v>
       </c>
-      <c r="T9" s="1">
+      <c r="U9" s="1">
         <v>42626</v>
       </c>
-      <c r="W9" s="1"/>
       <c r="X9" s="1"/>
-      <c r="Y9" s="3">
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="3">
         <v>0.1</v>
       </c>
-      <c r="Z9" s="3">
-        <v>0.9</v>
-      </c>
       <c r="AA9" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AB9" s="3">
         <v>120</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
         <v>48</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>58</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
         <v>42552</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>42686.833333333336</v>
       </c>
-      <c r="D10" s="3">
-        <v>24</v>
-      </c>
-      <c r="E10">
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>51</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>-18</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>4</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>16</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>5</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>300</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>30</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>1</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>2</v>
       </c>
-      <c r="N10">
-        <v>0.9</v>
-      </c>
       <c r="O10">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
         <v>1.4</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>8.6831499999999995</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>46.542630000000003</v>
       </c>
-      <c r="S10" s="1">
+      <c r="T10" s="1">
         <v>42552</v>
       </c>
-      <c r="T10" s="1">
+      <c r="U10" s="1">
         <v>42631</v>
       </c>
-      <c r="W10" s="1"/>
       <c r="X10" s="1"/>
-      <c r="Y10" s="3">
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="3">
         <v>0.1</v>
       </c>
-      <c r="Z10" s="3">
-        <v>0.9</v>
-      </c>
       <c r="AA10" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AB10" s="3">
         <v>120</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
         <v>49</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" t="s">
         <v>58</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AE10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
         <v>42552</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>42641.673611111109</v>
       </c>
-      <c r="D11" s="3">
-        <v>24</v>
-      </c>
-      <c r="E11">
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>51</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>-18</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>4</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>16</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>5</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>300</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>30</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>1</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>2</v>
       </c>
-      <c r="N11">
-        <v>0.9</v>
-      </c>
       <c r="O11">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
         <v>1.4</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>8.7298899999999993</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>46.548409999999997</v>
       </c>
-      <c r="S11" s="1">
+      <c r="T11" s="1">
         <v>42552</v>
       </c>
-      <c r="T11" s="1">
+      <c r="U11" s="1">
         <v>42633</v>
       </c>
-      <c r="W11" s="1"/>
       <c r="X11" s="1"/>
-      <c r="Y11" s="3">
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="3">
         <v>0.1</v>
       </c>
-      <c r="Z11" s="3">
-        <v>0.9</v>
-      </c>
       <c r="AA11" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AB11" s="3">
         <v>120</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>50</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AD11" t="s">
         <v>58</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
         <v>42552</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>42647.628472222219</v>
       </c>
-      <c r="D12" s="3">
-        <v>24</v>
-      </c>
-      <c r="E12">
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12">
         <v>51</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>-18</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>4</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>16</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>5</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>300</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>30</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>1</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>2</v>
       </c>
-      <c r="N12">
-        <v>0.9</v>
-      </c>
       <c r="O12">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
         <v>1.4</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>8.6868200000000009</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>46.548490000000001</v>
       </c>
-      <c r="S12" s="1">
+      <c r="T12" s="1">
         <v>42552</v>
       </c>
-      <c r="T12" s="1">
+      <c r="U12" s="1">
         <v>42633</v>
       </c>
-      <c r="W12" s="1"/>
       <c r="X12" s="1"/>
-      <c r="Y12" s="3">
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="3">
         <v>0.1</v>
       </c>
-      <c r="Z12" s="3">
-        <v>0.9</v>
-      </c>
       <c r="AA12" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AB12" s="3">
         <v>120</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AC12" t="s">
         <v>51</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
         <v>58</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1">
         <v>43313</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>43412.243055555555</v>
       </c>
-      <c r="D13" s="3">
-        <v>24</v>
-      </c>
-      <c r="E13">
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13">
         <v>51</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>-18</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>4</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>16</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>5</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>300</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>30</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>1</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>2</v>
       </c>
-      <c r="N13">
-        <v>0.9</v>
-      </c>
       <c r="O13">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
         <v>1.4</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>8.7033740000000002</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>46.550142999999998</v>
       </c>
-      <c r="S13" s="1">
+      <c r="T13" s="1">
         <v>43313</v>
       </c>
-      <c r="T13" s="1">
+      <c r="U13" s="1">
         <v>43354</v>
       </c>
-      <c r="W13" s="1"/>
       <c r="X13" s="1"/>
-      <c r="Y13" s="3">
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="3">
         <v>0.1</v>
       </c>
-      <c r="Z13" s="3">
-        <v>0.9</v>
-      </c>
       <c r="AA13" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AB13" s="3">
         <v>120</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AC13" t="s">
         <v>53</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AD13" t="s">
         <v>58</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AE13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
         <v>43313</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>43361.690972222219</v>
       </c>
-      <c r="D14" s="3">
-        <v>24</v>
-      </c>
-      <c r="E14">
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14">
         <v>51</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>-18</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>4</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>16</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>5</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>300</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>30</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>1</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>2</v>
       </c>
-      <c r="N14">
-        <v>0.9</v>
-      </c>
       <c r="O14">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
         <v>1.4</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>8.6909840000000003</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>46.553140999999997</v>
       </c>
-      <c r="S14" s="1">
+      <c r="T14" s="1">
         <v>43313</v>
       </c>
-      <c r="T14" s="1">
+      <c r="U14" s="1">
         <v>43358</v>
       </c>
-      <c r="W14" s="1"/>
       <c r="X14" s="1"/>
-      <c r="Y14" s="3">
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="3">
         <v>0.1</v>
       </c>
-      <c r="Z14" s="3">
-        <v>0.9</v>
-      </c>
       <c r="AA14" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AB14" s="3">
         <v>120</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AC14" t="s">
         <v>55</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AD14" t="s">
         <v>58</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AE14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
         <v>43678</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>43754.649305555555</v>
       </c>
-      <c r="D15" s="3">
-        <v>24</v>
-      </c>
-      <c r="E15">
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15">
         <v>51</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>-18</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>4</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>16</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>5</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>300</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>30</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>1</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>2</v>
       </c>
-      <c r="N15">
-        <v>0.9</v>
-      </c>
       <c r="O15">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
         <v>1.4</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>8.6922119999999996</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>46.554926999999999</v>
       </c>
-      <c r="S15" s="1">
+      <c r="T15" s="1">
         <v>43678</v>
       </c>
-      <c r="T15" s="1">
+      <c r="U15" s="1">
         <v>43724</v>
       </c>
-      <c r="W15" s="1"/>
       <c r="X15" s="1"/>
-      <c r="Y15" s="3">
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="3">
         <v>0.1</v>
       </c>
-      <c r="Z15" s="3">
-        <v>0.9</v>
-      </c>
       <c r="AA15" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AB15" s="3">
         <v>120</v>
       </c>
-      <c r="AB15" t="s">
+      <c r="AC15" t="s">
         <v>57</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="AD15" t="s">
         <v>58</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AE15" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>